<commit_message>
add new data by prefecture and week
</commit_message>
<xml_diff>
--- a/raw_data/All 2009, 2010 data by week and location.xlsx
+++ b/raw_data/All 2009, 2010 data by week and location.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -362,8 +363,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="#,##0_ "/>
-    <numFmt numFmtId="167" formatCode="0_ "/>
+    <numFmt numFmtId="164" formatCode="#,##0_ "/>
+    <numFmt numFmtId="165" formatCode="0_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -583,961 +584,961 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>

</xml_diff>